<commit_message>
Seitenaufrufe fertiggestellt. Zeiten aktualisiert
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
   <si>
     <t>Aktivitäten und To-dos</t>
   </si>
@@ -150,10 +150,31 @@
     <t>Content Analyse der RZ-Website Teil 1</t>
   </si>
   <si>
-    <t>Piwik-Analyse (Ebene 1 +2)</t>
+    <t>Letzte Aktualisierung: 10.07.2015</t>
   </si>
   <si>
-    <t>Letzte Aktualisierung: 08.07.2015</t>
+    <t>Analyse des SRS-Templates</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benedikt Häring, Johannes Vogl </t>
+  </si>
+  <si>
+    <t>SRS-Dokument erstellen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Besprechung der nächsten Projektschritte </t>
+  </si>
+  <si>
+    <t>Content Analyse der RZ-Website Teil 2</t>
+  </si>
+  <si>
+    <t>Piwik-Analyse (Seitenansichten: Ebene 3)</t>
+  </si>
+  <si>
+    <t>Piwik-Analyse (Seitenansichten: Ebene 1 +2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Piwik-Analyse (Seitenansichten Visualisierung) </t>
   </si>
 </sst>
 </file>
@@ -761,11 +782,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK27"/>
+  <dimension ref="A1:AMK33"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6"/>
@@ -3882,7 +3903,7 @@
     </row>
     <row r="5" spans="1:1024">
       <c r="A5" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -9220,7 +9241,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -9234,43 +9255,124 @@
     </row>
     <row r="25" spans="1:4" ht="31.2">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="C25" s="14">
-        <v>0.33333333333333331</v>
+        <v>6.9444444444444447E-4</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="31.2">
       <c r="A26" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="14">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="31.2">
+      <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="14">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="31.2">
+      <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B28" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C28" s="14">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="D28" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C29" s="14">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D29" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="31.2">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="14">
+        <v>3.4722222222222224E-4</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C32" s="14">
+        <v>1.0416666666666667E-3</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="14">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="D33" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
content analyse stunden eingetragen
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\redesign-ur-rz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabi\workspace\redesign-ur-rz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8490" tabRatio="988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="kategorien" localSheetId="2">#REF!</definedName>
     <definedName name="kategorien">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -770,9 +770,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="10.69921875"/>
+    <col min="1" max="1025" width="10.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -786,23 +786,23 @@
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41" style="1"/>
-    <col min="2" max="2" width="24.796875" style="1"/>
-    <col min="3" max="3" width="20.19921875" style="1"/>
-    <col min="4" max="4" width="27.69921875" style="1"/>
+    <col min="2" max="2" width="24.75" style="1"/>
+    <col min="3" max="3" width="20.25" style="1"/>
+    <col min="4" max="4" width="27.75" style="1"/>
     <col min="5" max="5" width="23.5" style="1"/>
-    <col min="6" max="6" width="23.69921875" style="1"/>
-    <col min="7" max="7" width="19.296875" style="1"/>
-    <col min="8" max="8" width="14.796875" style="1"/>
-    <col min="9" max="1025" width="23.69921875" style="1"/>
+    <col min="6" max="6" width="23.75" style="1"/>
+    <col min="7" max="7" width="19.25" style="1"/>
+    <col min="8" max="8" width="14.75" style="1"/>
+    <col min="9" max="1025" width="23.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="19.05" customHeight="1">
+    <row r="1" spans="1:1024" ht="19.149999999999999" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1828,7 +1828,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.95" customHeight="1">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.9" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -5957,7 +5957,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" ht="13.05" customHeight="1">
+    <row r="7" spans="1:1024" ht="13.15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6983,7 +6983,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" ht="21" hidden="1">
+    <row r="8" spans="1:1024" ht="20.25" hidden="1">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -8009,7 +8009,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" ht="21">
+    <row r="9" spans="1:1024" ht="20.25">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -9043,7 +9043,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" ht="31.2">
+    <row r="10" spans="1:1024">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -9071,7 +9071,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" ht="31.2">
+    <row r="12" spans="1:1024">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" ht="31.2">
+    <row r="13" spans="1:1024">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -9099,7 +9099,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" ht="31.2">
+    <row r="14" spans="1:1024">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -9127,7 +9127,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" ht="31.2">
+    <row r="16" spans="1:1024">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -9183,7 +9183,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="31.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -9197,7 +9197,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="31.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -9211,7 +9211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="31.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -9253,7 +9253,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.2">
+    <row r="25" spans="1:4" ht="31.5">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -9267,7 +9267,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -9281,7 +9281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -9295,7 +9295,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.2">
+    <row r="28" spans="1:4" ht="31.5">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -9323,7 +9323,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="31.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -9343,6 +9343,9 @@
       </c>
       <c r="B31" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="C31" s="14">
+        <v>2.0833333333333333E-3</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>31</v>
@@ -9393,16 +9396,16 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.69921875" style="1"/>
-    <col min="2" max="2" width="24.796875" style="1"/>
-    <col min="3" max="3" width="17.796875" style="1"/>
-    <col min="4" max="4" width="27.69921875" style="1"/>
+    <col min="1" max="1" width="33.75" style="1"/>
+    <col min="2" max="2" width="24.75" style="1"/>
+    <col min="3" max="3" width="17.75" style="1"/>
+    <col min="4" max="4" width="27.75" style="1"/>
     <col min="5" max="5" width="17.5" style="1"/>
-    <col min="6" max="6" width="36.19921875" style="1"/>
-    <col min="7" max="7" width="14.796875" style="1"/>
-    <col min="8" max="1025" width="23.69921875" style="1"/>
+    <col min="6" max="6" width="36.25" style="1"/>
+    <col min="7" max="7" width="14.75" style="1"/>
+    <col min="8" max="1025" width="23.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -10431,7 +10434,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="28.2">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="27.75">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -10535,7 +10538,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:1024" ht="21">
+    <row r="8" spans="1:1024" ht="20.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -10544,7 +10547,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:1024" ht="21">
+    <row r="9" spans="1:1024" ht="20.25">
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
srs 45 fertig und zeitverteilung update
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fabi\workspace\redesign-ur-rz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hase\Desktop\redesign-ur-rz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8490" tabRatio="988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
   <si>
     <t>Aktivitäten und To-dos</t>
   </si>
@@ -175,6 +175,12 @@
   </si>
   <si>
     <t xml:space="preserve">Piwik-Analyse (Seitenansichten Visualisierung) </t>
+  </si>
+  <si>
+    <t>SRS Template anpassen</t>
+  </si>
+  <si>
+    <t>SRS schreiben</t>
   </si>
 </sst>
 </file>
@@ -770,9 +776,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1025" width="10.75"/>
+    <col min="1" max="1025" width="10.69921875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -782,27 +788,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK33"/>
+  <dimension ref="A1:AMK35"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="41" style="1"/>
-    <col min="2" max="2" width="24.75" style="1"/>
-    <col min="3" max="3" width="20.25" style="1"/>
-    <col min="4" max="4" width="27.75" style="1"/>
+    <col min="2" max="2" width="24.69921875" style="1"/>
+    <col min="3" max="3" width="20.19921875" style="1"/>
+    <col min="4" max="4" width="27.69921875" style="1"/>
     <col min="5" max="5" width="23.5" style="1"/>
-    <col min="6" max="6" width="23.75" style="1"/>
-    <col min="7" max="7" width="19.25" style="1"/>
-    <col min="8" max="8" width="14.75" style="1"/>
-    <col min="9" max="1025" width="23.75" style="1"/>
+    <col min="6" max="6" width="23.69921875" style="1"/>
+    <col min="7" max="7" width="19.19921875" style="1"/>
+    <col min="8" max="8" width="14.69921875" style="1"/>
+    <col min="9" max="1025" width="23.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="19.149999999999999" customHeight="1">
+    <row r="1" spans="1:1024" ht="19.2" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1828,7 +1834,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.9" customHeight="1">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.95" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -5957,7 +5963,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" ht="13.15" customHeight="1">
+    <row r="7" spans="1:1024" ht="13.2" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6983,7 +6989,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" ht="20.25" hidden="1">
+    <row r="8" spans="1:1024" ht="21" hidden="1">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -8009,7 +8015,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" ht="20.25">
+    <row r="9" spans="1:1024" ht="21">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -9043,7 +9049,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024">
+    <row r="10" spans="1:1024" ht="31.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -9071,7 +9077,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1024">
+    <row r="12" spans="1:1024" ht="31.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -9085,7 +9091,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1024">
+    <row r="13" spans="1:1024" ht="31.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -9099,7 +9105,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:1024">
+    <row r="14" spans="1:1024" ht="31.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -9127,7 +9133,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1024">
+    <row r="16" spans="1:1024" ht="31.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -9183,7 +9189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="31.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -9197,7 +9203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="31.2">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -9211,7 +9217,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="31.2">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -9253,7 +9259,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5">
+    <row r="25" spans="1:4" ht="31.2">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -9267,7 +9273,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="31.2">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -9281,7 +9287,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="31.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -9295,7 +9301,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.5">
+    <row r="28" spans="1:4" ht="31.2">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -9323,7 +9329,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="31.2">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -9377,6 +9383,34 @@
       </c>
       <c r="D33" s="1" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="14">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="14">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -9396,16 +9430,16 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="33.75" style="1"/>
-    <col min="2" max="2" width="24.75" style="1"/>
-    <col min="3" max="3" width="17.75" style="1"/>
-    <col min="4" max="4" width="27.75" style="1"/>
+    <col min="1" max="1" width="33.69921875" style="1"/>
+    <col min="2" max="2" width="24.69921875" style="1"/>
+    <col min="3" max="3" width="17.69921875" style="1"/>
+    <col min="4" max="4" width="27.69921875" style="1"/>
     <col min="5" max="5" width="17.5" style="1"/>
-    <col min="6" max="6" width="36.25" style="1"/>
-    <col min="7" max="7" width="14.75" style="1"/>
-    <col min="8" max="1025" width="23.75" style="1"/>
+    <col min="6" max="6" width="36.19921875" style="1"/>
+    <col min="7" max="7" width="14.69921875" style="1"/>
+    <col min="8" max="1025" width="23.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -10434,7 +10468,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="27.75">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="28.2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -10538,7 +10572,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:1024" ht="20.25">
+    <row r="8" spans="1:1024" ht="21">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -10547,7 +10581,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:1024" ht="20.25">
+    <row r="9" spans="1:1024" ht="21">
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
zeiten in format hh:mm:ss angepasst
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hase\Desktop\redesign-ur-rz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\redesign-ur-rz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8490" tabRatio="988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -187,9 +187,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-  </numFmts>
   <fonts count="6">
     <font>
       <sz val="12"/>
@@ -283,7 +280,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -776,9 +773,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="10.69921875"/>
+    <col min="1" max="1025" width="10.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -790,25 +787,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK35"/>
   <sheetViews>
-    <sheetView windowProtection="1" tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+    <sheetView windowProtection="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41" style="1"/>
-    <col min="2" max="2" width="24.69921875" style="1"/>
-    <col min="3" max="3" width="20.19921875" style="1"/>
-    <col min="4" max="4" width="27.69921875" style="1"/>
+    <col min="2" max="2" width="24.75" style="1"/>
+    <col min="3" max="3" width="20.25" style="1"/>
+    <col min="4" max="4" width="27.75" style="1"/>
     <col min="5" max="5" width="23.5" style="1"/>
-    <col min="6" max="6" width="23.69921875" style="1"/>
-    <col min="7" max="7" width="19.19921875" style="1"/>
-    <col min="8" max="8" width="14.69921875" style="1"/>
-    <col min="9" max="1025" width="23.69921875" style="1"/>
+    <col min="6" max="6" width="23.75" style="1"/>
+    <col min="7" max="7" width="19.25" style="1"/>
+    <col min="8" max="8" width="14.75" style="1"/>
+    <col min="9" max="1025" width="23.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="19.2" customHeight="1">
+    <row r="1" spans="1:1024" ht="19.149999999999999" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1834,7 +1831,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.95" customHeight="1">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.9" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -5963,7 +5960,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" ht="13.2" customHeight="1">
+    <row r="7" spans="1:1024" ht="13.15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6989,7 +6986,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" ht="21" hidden="1">
+    <row r="8" spans="1:1024" ht="20.25" hidden="1">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -8015,7 +8012,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" ht="21">
+    <row r="9" spans="1:1024" ht="20.25">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -9049,7 +9046,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" ht="31.2">
+    <row r="10" spans="1:1024">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -9077,7 +9074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" ht="31.2">
+    <row r="12" spans="1:1024">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -9091,7 +9088,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" ht="31.2">
+    <row r="13" spans="1:1024">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -9105,7 +9102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" ht="31.2">
+    <row r="14" spans="1:1024">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -9133,7 +9130,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" ht="31.2">
+    <row r="16" spans="1:1024">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -9189,7 +9186,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="31.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -9203,7 +9200,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="31.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -9217,7 +9214,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="31.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -9239,7 +9236,7 @@
         <v>21</v>
       </c>
       <c r="C23" s="14">
-        <v>2.7777777777777779E-3</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>31</v>
@@ -9253,13 +9250,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="14">
-        <v>6.9444444444444447E-4</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.2">
+    <row r="25" spans="1:4" ht="31.5">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -9267,13 +9264,13 @@
         <v>41</v>
       </c>
       <c r="C25" s="14">
-        <v>6.9444444444444447E-4</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -9281,13 +9278,13 @@
         <v>20</v>
       </c>
       <c r="C26" s="14">
-        <v>6.9444444444444447E-4</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -9301,7 +9298,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.2">
+    <row r="28" spans="1:4" ht="31.5">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -9329,7 +9326,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="31.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -9337,7 +9334,7 @@
         <v>20</v>
       </c>
       <c r="C30" s="14">
-        <v>3.4722222222222224E-4</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
@@ -9351,7 +9348,7 @@
         <v>21</v>
       </c>
       <c r="C31" s="14">
-        <v>2.0833333333333333E-3</v>
+        <v>0.125</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>31</v>
@@ -9365,7 +9362,7 @@
         <v>23</v>
       </c>
       <c r="C32" s="14">
-        <v>1.0416666666666667E-3</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>31</v>
@@ -9379,7 +9376,7 @@
         <v>23</v>
       </c>
       <c r="C33" s="14">
-        <v>6.9444444444444447E-4</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>31</v>
@@ -9430,16 +9427,16 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.69921875" style="1"/>
-    <col min="2" max="2" width="24.69921875" style="1"/>
-    <col min="3" max="3" width="17.69921875" style="1"/>
-    <col min="4" max="4" width="27.69921875" style="1"/>
+    <col min="1" max="1" width="33.75" style="1"/>
+    <col min="2" max="2" width="24.75" style="1"/>
+    <col min="3" max="3" width="17.75" style="1"/>
+    <col min="4" max="4" width="27.75" style="1"/>
     <col min="5" max="5" width="17.5" style="1"/>
-    <col min="6" max="6" width="36.19921875" style="1"/>
-    <col min="7" max="7" width="14.69921875" style="1"/>
-    <col min="8" max="1025" width="23.69921875" style="1"/>
+    <col min="6" max="6" width="36.25" style="1"/>
+    <col min="7" max="7" width="14.75" style="1"/>
+    <col min="8" max="1025" width="23.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -10468,7 +10465,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="28.2">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="27.75">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -10572,7 +10569,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:1024" ht="21">
+    <row r="8" spans="1:1024" ht="20.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -10581,7 +10578,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:1024" ht="21">
+    <row r="9" spans="1:1024" ht="20.25">
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Piwik Seitentitel begonnen (1-5)
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\redesign-ur-rz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\redesign-ur-rz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8490" tabRatio="988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="52">
   <si>
     <t>Aktivitäten und To-dos</t>
   </si>
@@ -184,6 +184,9 @@
   </si>
   <si>
     <t>Alle Teammitglieder</t>
+  </si>
+  <si>
+    <t>Piwik-Analyse (Seitentitel 1-5)</t>
   </si>
 </sst>
 </file>
@@ -776,9 +779,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1025" width="10.75"/>
+    <col min="1" max="1025" width="10.69921875"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -788,27 +791,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK36"/>
+  <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37"/>
+      <pane ySplit="9" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="41" style="1"/>
-    <col min="2" max="2" width="24.75" style="1"/>
-    <col min="3" max="3" width="20.25" style="1"/>
-    <col min="4" max="4" width="27.75" style="1"/>
+    <col min="2" max="2" width="24.69921875" style="1"/>
+    <col min="3" max="3" width="20.19921875" style="1"/>
+    <col min="4" max="4" width="27.69921875" style="1"/>
     <col min="5" max="5" width="23.5" style="1"/>
-    <col min="6" max="6" width="23.75" style="1"/>
-    <col min="7" max="7" width="19.25" style="1"/>
-    <col min="8" max="8" width="14.75" style="1"/>
-    <col min="9" max="1025" width="23.75" style="1"/>
+    <col min="6" max="6" width="23.69921875" style="1"/>
+    <col min="7" max="7" width="19.19921875" style="1"/>
+    <col min="8" max="8" width="14.69921875" style="1"/>
+    <col min="9" max="1025" width="23.69921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="19.149999999999999" customHeight="1">
+    <row r="1" spans="1:1024" ht="19.2" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1834,7 +1837,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.9" customHeight="1">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.95" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -5963,7 +5966,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" ht="13.15" customHeight="1">
+    <row r="7" spans="1:1024" ht="13.2" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6989,7 +6992,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" ht="20.25" hidden="1">
+    <row r="8" spans="1:1024" ht="21" hidden="1">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -8015,7 +8018,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" ht="20.25">
+    <row r="9" spans="1:1024" ht="21">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -9049,7 +9052,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024">
+    <row r="10" spans="1:1024" ht="31.2">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -9077,7 +9080,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1024">
+    <row r="12" spans="1:1024" ht="31.2">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -9091,7 +9094,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1024">
+    <row r="13" spans="1:1024" ht="31.2">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -9105,7 +9108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:1024">
+    <row r="14" spans="1:1024" ht="31.2">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -9133,7 +9136,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1024">
+    <row r="16" spans="1:1024" ht="31.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -9189,7 +9192,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" ht="31.2">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -9203,7 +9206,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="31.2">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -9217,7 +9220,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" ht="31.2">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -9259,7 +9262,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.5">
+    <row r="25" spans="1:4" ht="31.2">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -9273,7 +9276,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="31.2">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -9287,7 +9290,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" ht="31.2">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -9301,7 +9304,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.5">
+    <row r="28" spans="1:4" ht="31.2">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -9329,7 +9332,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="31.2">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -9425,6 +9428,20 @@
       </c>
       <c r="D36" s="1" t="s">
         <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -9444,16 +9461,16 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="33.75" style="1"/>
-    <col min="2" max="2" width="24.75" style="1"/>
-    <col min="3" max="3" width="17.75" style="1"/>
-    <col min="4" max="4" width="27.75" style="1"/>
+    <col min="1" max="1" width="33.69921875" style="1"/>
+    <col min="2" max="2" width="24.69921875" style="1"/>
+    <col min="3" max="3" width="17.69921875" style="1"/>
+    <col min="4" max="4" width="27.69921875" style="1"/>
     <col min="5" max="5" width="17.5" style="1"/>
-    <col min="6" max="6" width="36.25" style="1"/>
-    <col min="7" max="7" width="14.75" style="1"/>
-    <col min="8" max="1025" width="23.75" style="1"/>
+    <col min="6" max="6" width="36.19921875" style="1"/>
+    <col min="7" max="7" width="14.69921875" style="1"/>
+    <col min="8" max="1025" width="23.69921875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -10482,7 +10499,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="27.75">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="28.2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -10586,7 +10603,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:1024" ht="20.25">
+    <row r="8" spans="1:1024" ht="21">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -10595,7 +10612,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:1024" ht="20.25">
+    <row r="9" spans="1:1024" ht="21">
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
stunden hinzugefügt korrekturen am srs
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hase\Desktop\redesign-ur-rz\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\workspace\redesign-ur-rz\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <workbookProtection lockWindows="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8496" tabRatio="988" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8490" tabRatio="988" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Allgemein" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="53">
   <si>
     <t>Aktivitäten und To-dos</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Piwik-Analyse (Seitentitel 1-5)</t>
+  </si>
+  <si>
+    <t>Dominik Bauer, Benedikt Häring, Fabian Huth</t>
   </si>
 </sst>
 </file>
@@ -779,9 +782,9 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1025" width="10.69921875"/>
+    <col min="1" max="1025" width="10.75"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -791,27 +794,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK39"/>
+  <dimension ref="A1:AMK40"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="41" style="1"/>
-    <col min="2" max="2" width="24.69921875" style="1"/>
-    <col min="3" max="3" width="20.19921875" style="1"/>
-    <col min="4" max="4" width="27.69921875" style="1"/>
+    <col min="2" max="2" width="24.75" style="1"/>
+    <col min="3" max="3" width="20.25" style="1"/>
+    <col min="4" max="4" width="27.75" style="1"/>
     <col min="5" max="5" width="23.5" style="1"/>
-    <col min="6" max="6" width="23.69921875" style="1"/>
-    <col min="7" max="7" width="19.19921875" style="1"/>
-    <col min="8" max="8" width="14.69921875" style="1"/>
-    <col min="9" max="1025" width="23.69921875" style="1"/>
+    <col min="6" max="6" width="23.75" style="1"/>
+    <col min="7" max="7" width="19.25" style="1"/>
+    <col min="8" max="8" width="14.75" style="1"/>
+    <col min="9" max="1025" width="23.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" ht="19.2" customHeight="1">
+    <row r="1" spans="1:1024" ht="19.149999999999999" customHeight="1">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1837,7 +1840,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.95" customHeight="1">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="97.9" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -5966,7 +5969,7 @@
       <c r="AMI6"/>
       <c r="AMJ6"/>
     </row>
-    <row r="7" spans="1:1024" ht="13.2" customHeight="1">
+    <row r="7" spans="1:1024" ht="13.15" customHeight="1">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -6992,7 +6995,7 @@
       <c r="AMI7"/>
       <c r="AMJ7"/>
     </row>
-    <row r="8" spans="1:1024" ht="21" hidden="1">
+    <row r="8" spans="1:1024" ht="20.25" hidden="1">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -8018,7 +8021,7 @@
       <c r="AMI8"/>
       <c r="AMJ8"/>
     </row>
-    <row r="9" spans="1:1024" ht="21">
+    <row r="9" spans="1:1024" ht="20.25">
       <c r="A9" s="13" t="s">
         <v>4</v>
       </c>
@@ -9052,7 +9055,7 @@
       <c r="AMI9"/>
       <c r="AMJ9"/>
     </row>
-    <row r="10" spans="1:1024" ht="31.2">
+    <row r="10" spans="1:1024">
       <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
@@ -9080,7 +9083,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:1024" ht="31.2">
+    <row r="12" spans="1:1024">
       <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
@@ -9094,7 +9097,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:1024" ht="31.2">
+    <row r="13" spans="1:1024">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -9108,7 +9111,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:1024" ht="31.2">
+    <row r="14" spans="1:1024">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -9136,7 +9139,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:1024" ht="31.2">
+    <row r="16" spans="1:1024">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -9192,7 +9195,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="31.2">
+    <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -9206,7 +9209,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="31.2">
+    <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>36</v>
       </c>
@@ -9220,7 +9223,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="31.2">
+    <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -9262,7 +9265,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="31.2">
+    <row r="25" spans="1:4" ht="31.5">
       <c r="A25" s="1" t="s">
         <v>40</v>
       </c>
@@ -9276,7 +9279,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.2">
+    <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>43</v>
       </c>
@@ -9290,7 +9293,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="31.2">
+    <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>37</v>
       </c>
@@ -9304,7 +9307,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.2">
+    <row r="28" spans="1:4" ht="31.5">
       <c r="A28" s="1" t="s">
         <v>34</v>
       </c>
@@ -9332,7 +9335,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="31.2">
+    <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>15</v>
       </c>
@@ -9458,7 +9461,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="31.2">
+    <row r="39" spans="1:4" ht="31.5">
       <c r="A39" s="1" t="s">
         <v>49</v>
       </c>
@@ -9469,6 +9472,20 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D39" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="31.5">
+      <c r="A40" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -9489,16 +9506,16 @@
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="33.69921875" style="1"/>
-    <col min="2" max="2" width="24.69921875" style="1"/>
-    <col min="3" max="3" width="17.69921875" style="1"/>
-    <col min="4" max="4" width="27.69921875" style="1"/>
+    <col min="1" max="1" width="33.75" style="1"/>
+    <col min="2" max="2" width="24.75" style="1"/>
+    <col min="3" max="3" width="17.75" style="1"/>
+    <col min="4" max="4" width="27.75" style="1"/>
     <col min="5" max="5" width="17.5" style="1"/>
-    <col min="6" max="6" width="36.19921875" style="1"/>
-    <col min="7" max="7" width="14.69921875" style="1"/>
-    <col min="8" max="1025" width="23.69921875" style="1"/>
+    <col min="6" max="6" width="36.25" style="1"/>
+    <col min="7" max="7" width="14.75" style="1"/>
+    <col min="8" max="1025" width="23.75" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1024">
@@ -10527,7 +10544,7 @@
       <c r="AMI1"/>
       <c r="AMJ1"/>
     </row>
-    <row r="2" spans="1:1024" s="7" customFormat="1" ht="28.2">
+    <row r="2" spans="1:1024" s="7" customFormat="1" ht="27.75">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -10631,7 +10648,7 @@
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
     </row>
-    <row r="8" spans="1:1024" ht="21">
+    <row r="8" spans="1:1024" ht="20.25">
       <c r="A8" s="12"/>
       <c r="B8" s="12"/>
       <c r="C8" s="12"/>
@@ -10640,7 +10657,7 @@
       <c r="F8" s="12"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="1:1024" ht="21">
+    <row r="9" spans="1:1024" ht="20.25">
       <c r="A9" s="13" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Zeit Update und Card sorting
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="74">
   <si>
     <t>Aktivitäten und To-dos</t>
   </si>
@@ -247,6 +247,12 @@
   </si>
   <si>
     <t>Dominik Bauer, Benedikt Häring, Johannes Vogl</t>
+  </si>
+  <si>
+    <t>Card Sorting Begriffe</t>
+  </si>
+  <si>
+    <t>Card Sorting Concept Codify</t>
   </si>
 </sst>
 </file>
@@ -851,11 +857,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK56"/>
+  <dimension ref="A1:AMK58"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D56" sqref="D56"/>
+      <pane ySplit="9" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
@@ -9707,6 +9713,9 @@
       <c r="B52" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="C52" s="14">
+        <v>0.16666666666666666</v>
+      </c>
       <c r="D52" s="1" t="s">
         <v>31</v>
       </c>
@@ -9764,6 +9773,34 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D56" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="31.2">
+      <c r="A57" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C57" s="14">
+        <v>0.125</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C58" s="14">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update Projektplan und Zeiten aktualisiert
</commit_message>
<xml_diff>
--- a/Arbeitsaufgaben_und_Aktivitäten.xlsx
+++ b/Arbeitsaufgaben_und_Aktivitäten.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="79">
   <si>
     <t>Aktivitäten und To-dos</t>
   </si>
@@ -195,9 +195,6 @@
     <t xml:space="preserve">Projektplanung </t>
   </si>
   <si>
-    <t>Letzte Aktualisierung: 20.07.2015</t>
-  </si>
-  <si>
     <t>SRS Update</t>
   </si>
   <si>
@@ -240,9 +237,6 @@
     <t>Projektdokumentation</t>
   </si>
   <si>
-    <t>Anforderungsanalyse</t>
-  </si>
-  <si>
     <t>Fragebogen überarbeiten</t>
   </si>
   <si>
@@ -265,6 +259,15 @@
   </si>
   <si>
     <t>Update des Projektplans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erstellen einer Sitemap der aktuellen RZ-Seite </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benedikt Häring, Fabian Huth, Johannes Vogl </t>
+  </si>
+  <si>
+    <t>Letzte Aktualisierung: 31.08.2015</t>
   </si>
 </sst>
 </file>
@@ -869,11 +872,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK67"/>
+  <dimension ref="A1:AMK70"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B73" sqref="B73"/>
+      <pane ySplit="9" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.69921875" defaultRowHeight="15.6"/>
@@ -3990,7 +3993,7 @@
     </row>
     <row r="5" spans="1:1024">
       <c r="A5" s="8" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -9286,10 +9289,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="14">
         <v>8.3333333333333329E-2</v>
@@ -9328,7 +9331,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -9340,15 +9343,15 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" ht="31.2">
       <c r="A25" s="1" t="s">
-        <v>38</v>
+        <v>76</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="C25" s="14">
-        <v>0.16666666666666666</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>31</v>
@@ -9356,111 +9359,111 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C26" s="14">
-        <v>1.0416666666666666E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C27" s="14">
-        <v>4.1666666666666664E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="31.2">
+    <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C28" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="31.2">
       <c r="A29" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C29" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" ht="31.2">
       <c r="A30" s="1" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C30" s="14">
-        <v>1.0416666666666666E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="31.2">
+    <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
-        <v>37</v>
+        <v>75</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C31" s="14">
-        <v>0.33333333333333331</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="31.2">
       <c r="A32" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="C32" s="14">
-        <v>0.16666666666666666</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" ht="31.2">
       <c r="A33" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C33" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>31</v>
@@ -9468,55 +9471,55 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
-        <v>77</v>
+        <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="14">
+      <c r="C35" s="14">
         <v>1.0416666666666666E-2</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="31.2">
-      <c r="A35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C35" s="14">
-        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="31.2">
       <c r="A36" s="1" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C36" s="14">
-        <v>0.125</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C37" s="14">
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>31</v>
@@ -9524,13 +9527,13 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C38" s="14">
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>31</v>
@@ -9538,27 +9541,27 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C39" s="14">
-        <v>1.0416666666666666E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="14">
-        <v>0.16666666666666666</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>27</v>
@@ -9566,13 +9569,13 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>24</v>
       </c>
       <c r="C41" s="14">
-        <v>0.29166666666666669</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>27</v>
@@ -9583,10 +9586,10 @@
         <v>48</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C42" s="14">
-        <v>0.16666666666666666</v>
+        <v>0.29166666666666669</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>27</v>
@@ -9594,41 +9597,41 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="C43" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C44" s="14">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="31.2">
+    <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C45" s="14">
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>27</v>
@@ -9639,7 +9642,7 @@
         <v>48</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C46" s="14">
         <v>4.1666666666666664E-2</v>
@@ -9650,41 +9653,41 @@
     </row>
     <row r="47" spans="1:4" ht="31.2">
       <c r="A47" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>20</v>
+        <v>51</v>
       </c>
       <c r="C47" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="31.2">
       <c r="A48" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C48" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="31.2">
+      <c r="A49" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="14">
         <v>4.1666666666666664E-2</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C49" s="14">
-        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>27</v>
@@ -9692,13 +9695,13 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="C50" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>27</v>
@@ -9706,7 +9709,7 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>49</v>
@@ -9715,46 +9718,46 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C52" s="14">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="31.2">
+    <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
-        <v>57</v>
+        <v>75</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="C53" s="14">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C54" s="14">
-        <v>4.1666666666666664E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>31</v>
@@ -9762,41 +9765,41 @@
     </row>
     <row r="55" spans="1:4" ht="31.2">
       <c r="A55" s="1" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C55" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>0.125</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="31.2">
+    <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C56" s="14">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="31.2">
       <c r="A57" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>20</v>
       </c>
       <c r="C57" s="14">
-        <v>0.33333333333333331</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>31</v>
@@ -9807,94 +9810,94 @@
         <v>64</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="C58" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" ht="31.2">
       <c r="A59" s="1" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C59" s="14">
-        <v>1.0416666666666666E-2</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D59" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="31.2">
+      <c r="A60" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C60" s="14">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
-      <c r="A60" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C60" s="14">
-        <v>0.16666666666666666</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C61" s="14">
-        <v>8.3333333333333329E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C62" s="14">
-        <v>4.1666666666666664E-2</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B63" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C63" s="14">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B64" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C63" s="14">
+      <c r="C64" s="14">
         <v>0.125</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="31.2">
-      <c r="A64" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C64" s="14">
-        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>31</v>
@@ -9902,27 +9905,27 @@
     </row>
     <row r="65" spans="1:4" ht="31.2">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>32</v>
+        <v>69</v>
       </c>
       <c r="C65" s="14">
-        <v>0.125</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" ht="31.2">
       <c r="A66" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="C66" s="14">
-        <v>0.20833333333333334</v>
+        <v>0.125</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>31</v>
@@ -9930,15 +9933,55 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B67" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" s="14">
+        <v>0.20833333333333334</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B68" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C67" s="14">
+      <c r="C68" s="14">
         <v>1.0416666666666666E-2</v>
       </c>
-      <c r="D67" s="1" t="s">
+      <c r="D68" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C69" s="14"/>
+      <c r="D69" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C70" s="14">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>